<commit_message>
Improving table and reversing color scale
</commit_message>
<xml_diff>
--- a/app/Survey_info.xlsx
+++ b/app/Survey_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\stations\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704A4DD8-FCB3-44D6-AB9F-04A9F3276D1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22BAD317-4E4C-4351-AD4E-901AD0E48648}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{093C89F6-4872-4273-9605-AB3AAE5AC5BB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="80">
   <si>
     <t>Survey</t>
   </si>
@@ -221,17 +221,65 @@
     <t xml:space="preserve">https://portal.edirepository.org/nis/metadataviewer?packageid=edi.494.1; </t>
   </si>
   <si>
-    <t>Link 1</t>
-  </si>
-  <si>
-    <t>Link 2</t>
+    <t>Survey_link</t>
+  </si>
+  <si>
+    <t>https://iep.ca.gov/Science-Synthesis-Service/Monitoring-Programs/20-mm</t>
+  </si>
+  <si>
+    <t>https://iep.ca.gov/Science-Synthesis-Service/Monitoring-Programs/Delta-Juvenile-Fish</t>
+  </si>
+  <si>
+    <t>https://iep.ca.gov/Science-Synthesis-Service/Monitoring-Programs/EMP</t>
+  </si>
+  <si>
+    <t>https://iep.ca.gov/Science-Synthesis-Service/Monitoring-Programs/Fall-Midwater-Trawl</t>
+  </si>
+  <si>
+    <t>https://iep.ca.gov/Science-Synthesis-Service/Monitoring-Programs/Spring-Kodiak</t>
+  </si>
+  <si>
+    <t>https://iep.ca.gov/Science-Synthesis-Service/Monitoring-Programs/Suisun-Marsh</t>
+  </si>
+  <si>
+    <t>https://iep.ca.gov/Science-Synthesis-Service/Monitoring-Programs/Summer-Townet</t>
+  </si>
+  <si>
+    <t>https://iep.ca.gov/Science-Synthesis-Service/Monitoring-Programs/Yolo-Bypass</t>
+  </si>
+  <si>
+    <t>Data source 1</t>
+  </si>
+  <si>
+    <t>Data source 2</t>
+  </si>
+  <si>
+    <t>http://www.dfg.ca.gov/delta/projects.asp?ProjectID=BAYSTUDY</t>
+  </si>
+  <si>
+    <t>https://sfbay.wr.usgs.gov/access/wqdata/index.html</t>
+  </si>
+  <si>
+    <t>FTP</t>
+  </si>
+  <si>
+    <t>EDI</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>ScienceBase</t>
+  </si>
+  <si>
+    <t>Data_source_name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,6 +297,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -275,7 +329,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -287,6 +341,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -602,355 +657,432 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35511161-FE4A-4A26-88E8-411A4A27DC4E}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="71.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>1995</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>1976</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>2016</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>1975</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>1967</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <v>2016</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>33</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>7</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>2012</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>1980</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>1969</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J10" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>2002</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <v>1979</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="1">
+      <c r="E13" s="1">
         <v>1959</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="2">
+      <c r="E14" s="2">
         <v>1998</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J14" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F14">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G14">
     <sortCondition ref="A2:A14"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="G10" r:id="rId1" xr:uid="{85BC00A5-11DB-406F-8F28-CDF890BAD946}"/>
-    <hyperlink ref="G14" r:id="rId2" xr:uid="{CF3A6B37-4E56-4012-A682-82C2109C5925}"/>
+    <hyperlink ref="H10" r:id="rId1" xr:uid="{85BC00A5-11DB-406F-8F28-CDF890BAD946}"/>
+    <hyperlink ref="H14" r:id="rId2" xr:uid="{CF3A6B37-4E56-4012-A682-82C2109C5925}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Changed overall sampling effort metric to max across all parameters
</commit_message>
<xml_diff>
--- a/app/Survey_info.xlsx
+++ b/app/Survey_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\stations\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22BAD317-4E4C-4351-AD4E-901AD0E48648}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944A640F-EB76-4752-BA16-5A352F982737}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{093C89F6-4872-4273-9605-AB3AAE5AC5BB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="82">
   <si>
     <t>Survey</t>
   </si>
@@ -273,6 +273,12 @@
   </si>
   <si>
     <t>Data_source_name</t>
+  </si>
+  <si>
+    <t>https://iep.ca.gov/Science-Synthesis-Service/Monitoring-Programs/Tidal-Wetland</t>
+  </si>
+  <si>
+    <t>https://www.fws.gov/lodi/juvenile_fish_monitoring_program/jfmp_index.htm</t>
   </si>
 </sst>
 </file>
@@ -329,7 +335,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -342,6 +348,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -660,7 +669,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,7 +776,9 @@
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="4" t="s">
+        <v>81</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>38</v>
       </c>
@@ -852,7 +863,9 @@
       <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="6" t="s">
+        <v>80</v>
+      </c>
       <c r="C7" s="2" t="s">
         <v>40</v>
       </c>
@@ -1083,8 +1096,10 @@
   <hyperlinks>
     <hyperlink ref="H10" r:id="rId1" xr:uid="{85BC00A5-11DB-406F-8F28-CDF890BAD946}"/>
     <hyperlink ref="H14" r:id="rId2" xr:uid="{CF3A6B37-4E56-4012-A682-82C2109C5925}"/>
+    <hyperlink ref="B7" r:id="rId3" xr:uid="{3D800910-B816-47D9-A50F-28D5E1AB21CC}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{64C330CB-F0E6-40A9-A3A9-3DEB23165807}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding Smelt Larva Survey
</commit_message>
<xml_diff>
--- a/app/Survey_info.xlsx
+++ b/app/Survey_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\stations\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944A640F-EB76-4752-BA16-5A352F982737}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8C243B-86B8-4AAC-B053-5A7AB4954EF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{093C89F6-4872-4273-9605-AB3AAE5AC5BB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="87">
   <si>
     <t>Survey</t>
   </si>
@@ -279,6 +279,21 @@
   </si>
   <si>
     <t>https://www.fws.gov/lodi/juvenile_fish_monitoring_program/jfmp_index.htm</t>
+  </si>
+  <si>
+    <t>SLS</t>
+  </si>
+  <si>
+    <t>Jan-Mar</t>
+  </si>
+  <si>
+    <t>https://portal.edirepository.org/nis/mapbrowse?packageid=edi.534.2</t>
+  </si>
+  <si>
+    <t>https://iep.ca.gov/Science-Synthesis-Service/Monitoring-Programs/Smelt-Larva</t>
+  </si>
+  <si>
+    <t>Smelt Larva Survey</t>
   </si>
 </sst>
 </file>
@@ -666,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35511161-FE4A-4A26-88E8-411A4A27DC4E}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,6 +1104,35 @@
         <v>56</v>
       </c>
     </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="2">
+        <v>2009</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" t="s">
+        <v>84</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G14">
     <sortCondition ref="A2:A14"/>

</xml_diff>

<commit_message>
Added more agencies to EMP
</commit_message>
<xml_diff>
--- a/app/Survey_info.xlsx
+++ b/app/Survey_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\stations\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C892CD-7317-46B6-B7E5-B54AFEFAB425}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5363277E-76AC-48CA-9FDE-CDF7FB73A681}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{093C89F6-4872-4273-9605-AB3AAE5AC5BB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="88">
   <si>
     <t>Survey</t>
   </si>
@@ -294,6 +294,9 @@
   </si>
   <si>
     <t>SFBS</t>
+  </si>
+  <si>
+    <t>California Department of Water Resources, California Department of Fish and Wildlife, United States Bureau of Reclamation</t>
   </si>
 </sst>
 </file>
@@ -684,7 +687,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,7 +830,7 @@
         <v>39</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="E5" s="1">
         <v>1975</v>

</xml_diff>

<commit_message>
Correcting 20mm frequency and adding improved sample effort filter
</commit_message>
<xml_diff>
--- a/app/Survey_info.xlsx
+++ b/app/Survey_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\stations\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5363277E-76AC-48CA-9FDE-CDF7FB73A681}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8628EE6-D478-4923-9923-1AE5D889FDD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{093C89F6-4872-4273-9605-AB3AAE5AC5BB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="89">
   <si>
     <t>Survey</t>
   </si>
@@ -297,6 +297,9 @@
   </si>
   <si>
     <t>California Department of Water Resources, California Department of Fish and Wildlife, United States Bureau of Reclamation</t>
+  </si>
+  <si>
+    <t>Every 2 weeks</t>
   </si>
 </sst>
 </file>
@@ -687,7 +690,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,7 +755,7 @@
         <v>14</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="H2" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Updating STN and SLS sampling frequency and fixing map legend
</commit_message>
<xml_diff>
--- a/app/Survey_info.xlsx
+++ b/app/Survey_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\stations\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8628EE6-D478-4923-9923-1AE5D889FDD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B40937-3C21-463A-8A30-F2FCBF693412}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{093C89F6-4872-4273-9605-AB3AAE5AC5BB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="88">
   <si>
     <t>Survey</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>Jun-Aug</t>
-  </si>
-  <si>
-    <t>2X monthly</t>
   </si>
   <si>
     <t>Spring Kodiak Trawl</t>
@@ -690,7 +687,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,10 +705,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -726,129 +723,129 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="1">
         <v>1995</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" s="1">
         <v>1976</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" s="1">
         <v>2016</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="H4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E5" s="1">
         <v>1975</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -856,13 +853,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" s="1">
         <v>1967</v>
@@ -874,57 +871,57 @@
         <v>7</v>
       </c>
       <c r="H6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" s="2">
         <v>2016</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G7" t="s">
         <v>7</v>
       </c>
       <c r="H7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="1">
         <v>2012</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>7</v>
@@ -932,121 +929,121 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9" s="1">
         <v>1980</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="1">
         <v>1969</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J10" t="s">
         <v>57</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="J10" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E11" s="1">
         <v>2002</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E12" s="1">
         <v>1979</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1054,13 +1051,13 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="1">
         <v>1959</v>
@@ -1069,74 +1066,74 @@
         <v>9</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="H13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E14" s="2">
         <v>1998</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E15" s="2">
         <v>2009</v>
       </c>
       <c r="F15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H15" t="s">
         <v>81</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" t="s">
-        <v>82</v>
-      </c>
       <c r="I15" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>